<commit_message>
ruleExtraction and showRule added
</commit_message>
<xml_diff>
--- a/results/TitanicHakankBinary/1/chars_of_network.xlsx
+++ b/results/TitanicHakankBinary/1/chars_of_network.xlsx
@@ -19,7 +19,7 @@
     <t>CHARACTERISTICS OF THE TRAINED NETWORK</t>
   </si>
   <si>
-    <t>HIDDEN NODES: [6, 12, 7, 2, 2]</t>
+    <t>HIDDEN NODES: [5, 1]</t>
   </si>
   <si>
     <t>TRAINING CHARACTERISTICS</t>
@@ -28,7 +28,7 @@
     <t>Average standard deviation from center:</t>
   </si>
   <si>
-    <t>0.38724376261234283</t>
+    <t>0.3433964252471924</t>
   </si>
   <si>
     <t>Porcentage zero weights:</t>
@@ -55,25 +55,25 @@
     <t>Train</t>
   </si>
   <si>
-    <t>0.779291553133515</t>
-  </si>
-  <si>
-    <t>0.728744939271255</t>
-  </si>
-  <si>
-    <t>0.5056179775280899</t>
+    <t>0.6857402361489555</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>0.028089887640449437</t>
   </si>
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>0.7727272727272727</t>
-  </si>
-  <si>
-    <t>0.7354260089686099</t>
-  </si>
-  <si>
-    <t>0.4619718309859155</t>
+    <t>0.6836363636363636</t>
+  </si>
+  <si>
+    <t>0.7692307692307693</t>
+  </si>
+  <si>
+    <t>0.028169014084507043</t>
   </si>
 </sst>
 </file>

</xml_diff>